<commit_message>
Added cannibalized-not-ac-min SourceFirst and test
</commit_message>
<xml_diff>
--- a/resources/with_cannibals.xlsx
+++ b/resources/with_cannibals.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PolicyRecords" sheetId="1" state="visible" r:id="rId2"/>
@@ -1053,7 +1053,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.3359375" defaultRowHeight="12.3" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.35546875" defaultRowHeight="12.3" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.44"/>
@@ -5746,7 +5746,7 @@
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.3" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.3" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -5873,7 +5873,7 @@
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.3" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.3" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.56"/>
@@ -6081,14 +6081,15 @@
   </sheetPr>
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.16"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="11.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="11.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="15.61"/>
   </cols>
@@ -6273,14 +6274,14 @@
   </sheetPr>
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="11.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="11.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="73.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="41.68"/>
   </cols>

</xml_diff>